<commit_message>
Added Multiple Configuration & Util Files 2
</commit_message>
<xml_diff>
--- a/TestData/Userdata.xlsx
+++ b/TestData/Userdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91798\eclipse-workspace\TestProjectFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870B041A-0FA7-4B84-B752-28F5E69E5AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E669D29D-17FF-4A4E-A08C-90D7C4668F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>SuperAdmin</t>
   </si>
   <si>
@@ -46,15 +43,6 @@
   </si>
   <si>
     <t>admin123</t>
-  </si>
-  <si>
-    <t>admin345</t>
-  </si>
-  <si>
-    <t>Adminsfds</t>
-  </si>
-  <si>
-    <t>Adminfsdfsdf</t>
   </si>
 </sst>
 </file>
@@ -379,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,50 +391,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>